<commit_message>
scorpiomwA has been added to firmware release checklist.
git-svn-id: http://einstein/svn/firmware/FIR-00251-Proc/trunk@18468 3e98269d-ff51-e449-abca-491a6567d830
</commit_message>
<xml_diff>
--- a/bin/FirmwareReleaseChecklist.xlsx
+++ b/bin/FirmwareReleaseChecklist.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>Output</t>
   </si>
@@ -119,6 +119,9 @@
   </si>
   <si>
     <t>Commit release</t>
+  </si>
+  <si>
+    <t>Proc_scorpiomwA (12)</t>
   </si>
 </sst>
 </file>
@@ -296,6 +299,36 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -313,36 +346,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -645,10 +648,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q21"/>
+  <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -662,52 +665,52 @@
       <c r="A1" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="I1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="J1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="K1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="23" t="s">
+      <c r="L1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="23" t="s">
+      <c r="M1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="23" t="s">
+      <c r="N1" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="O1" s="23" t="s">
+      <c r="O1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="23" t="s">
+      <c r="P1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="23" t="s">
+      <c r="Q1" s="8" t="s">
         <v>17</v>
       </c>
     </row>
@@ -716,42 +719,42 @@
         <v>0</v>
       </c>
       <c r="B2" s="4"/>
-      <c r="C2" s="14"/>
+      <c r="C2" s="9"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="5"/>
       <c r="G2" s="2"/>
-      <c r="H2" s="14"/>
+      <c r="H2" s="9"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="14"/>
+      <c r="J2" s="9"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="5"/>
-      <c r="O2" s="16"/>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="18"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="13"/>
     </row>
     <row r="3" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="4"/>
-      <c r="C3" s="15"/>
+      <c r="C3" s="10"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="5"/>
       <c r="G3" s="2"/>
-      <c r="H3" s="15"/>
+      <c r="H3" s="10"/>
       <c r="I3" s="2"/>
-      <c r="J3" s="15"/>
+      <c r="J3" s="10"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="5"/>
-      <c r="O3" s="19"/>
-      <c r="P3" s="20"/>
-      <c r="Q3" s="21"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="16"/>
     </row>
     <row r="4" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -761,15 +764,15 @@
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="8"/>
+      <c r="F4" s="18"/>
       <c r="G4" s="6"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="14"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="9"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
-      <c r="N4" s="8"/>
+      <c r="N4" s="18"/>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
@@ -782,15 +785,15 @@
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="9"/>
+      <c r="F5" s="19"/>
       <c r="G5" s="6"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="17"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
-      <c r="N5" s="9"/>
+      <c r="N5" s="19"/>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
@@ -803,15 +806,15 @@
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="9"/>
+      <c r="F6" s="19"/>
       <c r="G6" s="6"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="17"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
-      <c r="N6" s="9"/>
+      <c r="N6" s="19"/>
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
@@ -824,15 +827,15 @@
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="9"/>
+      <c r="F7" s="19"/>
       <c r="G7" s="6"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="17"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
-      <c r="N7" s="9"/>
+      <c r="N7" s="19"/>
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
@@ -845,15 +848,15 @@
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="9"/>
+      <c r="F8" s="19"/>
       <c r="G8" s="6"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="17"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
-      <c r="N8" s="9"/>
+      <c r="N8" s="19"/>
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
@@ -866,15 +869,15 @@
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="9"/>
+      <c r="F9" s="19"/>
       <c r="G9" s="6"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="17"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
-      <c r="N9" s="9"/>
+      <c r="N9" s="19"/>
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
@@ -887,15 +890,15 @@
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="9"/>
+      <c r="F10" s="19"/>
       <c r="G10" s="6"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="17"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
-      <c r="N10" s="9"/>
+      <c r="N10" s="19"/>
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
@@ -908,81 +911,102 @@
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="9"/>
+      <c r="F11" s="19"/>
       <c r="G11" s="6"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="17"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
-      <c r="N11" s="9"/>
+      <c r="N11" s="19"/>
       <c r="O11" s="2"/>
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
     </row>
     <row r="12" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="10"/>
+      <c r="F12" s="19"/>
       <c r="G12" s="6"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="15"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="17"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
-      <c r="N12" s="10"/>
+      <c r="N12" s="19"/>
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="2"/>
+    <row r="13" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="20"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B16" s="2"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" s="2"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18" s="2"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19" s="2"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B20" s="2"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="2"/>
+      <c r="B22" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -990,10 +1014,10 @@
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="J2:J3"/>
     <mergeCell ref="O2:Q3"/>
-    <mergeCell ref="I4:I12"/>
-    <mergeCell ref="N4:N12"/>
-    <mergeCell ref="F4:F12"/>
-    <mergeCell ref="H4:H12"/>
+    <mergeCell ref="I4:I13"/>
+    <mergeCell ref="N4:N13"/>
+    <mergeCell ref="F4:F13"/>
+    <mergeCell ref="H4:H13"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>